<commit_message>
Add reset methods to combat systems for cleanup
Introduced Reset() methods to AbilitySystem, ActorFactory, EffectSystem, BuffSystem, MovementSystem, ViewSystem, and RuntimeIdAllocator to clear internal state. CombatManager now calls these resets on InGameExit, and GameManager triggers cleanup on exit. This ensures proper cleanup of combat-related data between game sessions.
</commit_message>
<xml_diff>
--- a/GameConfigs/Datas/#game.config.xlsx
+++ b/GameConfigs/Datas/#game.config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\ModularSurvivor\GameConfigs\Datas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\projects\ModularSurvivor\GameConfigs\Datas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A2F6E0-F111-448E-8997-805A982BD3A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F851E26-28EE-4277-A5DA-107C50EC5576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{53B3FBB6-B116-408D-BCC0-737AAAC6C9D0}"/>
+    <workbookView xWindow="4920" yWindow="3195" windowWidth="28800" windowHeight="15345" xr2:uid="{53B3FBB6-B116-408D-BCC0-737AAAC6C9D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -169,7 +169,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -185,7 +185,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -484,7 +484,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>